<commit_message>
Seamless file reader and parser from metadata
</commit_message>
<xml_diff>
--- a/source/metadata/patient_labels_kaveli.xlsx
+++ b/source/metadata/patient_labels_kaveli.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jauhiaim\OneDrive - TTY-saatio\TTY\KÄVELI\MITTAUSTULOKSET\shared_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzhu/[PROJECTS]/Parkinsons/PREP2018/Matlab_code/source/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A984642-15A9-E443-814B-902705435679}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>kav001</t>
   </si>
@@ -117,14 +118,17 @@
   </si>
   <si>
     <t>Patient in wheelchair or bedrest, dependent of others help</t>
+  </si>
+  <si>
+    <t>Walking Tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -163,7 +167,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,22 +447,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G13" sqref="G13:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -477,8 +482,11 @@
       <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -491,8 +499,11 @@
       <c r="F2" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -505,8 +516,11 @@
       <c r="F3" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -525,8 +539,11 @@
       <c r="F4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -539,8 +556,11 @@
       <c r="F5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -553,8 +573,11 @@
       <c r="F6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -567,8 +590,11 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -581,8 +607,11 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -595,8 +624,11 @@
       <c r="F9" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -609,8 +641,11 @@
       <c r="F10" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -623,8 +658,11 @@
       <c r="F11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -637,8 +675,11 @@
       <c r="F12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -651,8 +692,11 @@
       <c r="F13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -665,8 +709,11 @@
       <c r="F14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>21</v>
       </c>
@@ -674,7 +721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" s="5">
         <v>0</v>
       </c>
@@ -682,7 +729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" s="5">
         <v>1</v>
       </c>
@@ -690,7 +737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" s="5">
         <v>1.5</v>
       </c>
@@ -698,7 +745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" s="5">
         <v>2</v>
       </c>
@@ -706,7 +753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" s="5">
         <v>2.5</v>
       </c>
@@ -714,7 +761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" s="5">
         <v>3</v>
       </c>
@@ -722,7 +769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" s="5">
         <v>4</v>
       </c>
@@ -730,7 +777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" s="5">
         <v>5</v>
       </c>

</xml_diff>